<commit_message>
Assignment of day 41
</commit_message>
<xml_diff>
--- a/seleniumwebdriver/testdate/caldata.xlsx
+++ b/seleniumwebdriver/testdate/caldata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="19095" windowHeight="4125"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15645" windowHeight="3300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1:P4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="21">
   <si>
     <t>Principle</t>
   </si>
@@ -58,6 +59,27 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>Initial Deposit Amount</t>
+  </si>
+  <si>
+    <t>Length(Months)</t>
+  </si>
+  <si>
+    <t>Interest rate</t>
+  </si>
+  <si>
+    <t>compounding</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Compounded Monthly</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -74,7 +96,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -82,23 +104,33 @@
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
-      <patternFill patternType="none">
+      <patternFill patternType="solid">
         <bgColor indexed="17"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <bgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
         <bgColor indexed="10"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <bgColor indexed="10"/>
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
       </patternFill>
     </fill>
   </fills>
@@ -114,13 +146,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,7 +455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -474,7 +512,7 @@
       <c r="G2" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="H2" t="s" s="1">
+      <c r="H2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -500,7 +538,7 @@
       <c r="G3" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="H3" t="s" s="2">
+      <c r="H3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -526,7 +564,7 @@
       <c r="G4" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="H4" t="s" s="3">
+      <c r="H4" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -552,7 +590,7 @@
       <c r="G5" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="H5" t="s" s="4">
+      <c r="H5" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -578,7 +616,7 @@
       <c r="G6" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="H6" t="s" s="5">
+      <c r="H6" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -589,12 +627,150 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.42578125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.28515625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="21.140625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="0">
+        <v>500</v>
+      </c>
+      <c r="B2" s="0">
+        <v>2</v>
+      </c>
+      <c r="C2" s="0">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E2" s="0">
+        <v>520.39</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s" s="10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="0">
+        <v>1000</v>
+      </c>
+      <c r="B3" s="0">
+        <v>4</v>
+      </c>
+      <c r="C3" s="0">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1083.1400000000001</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="0">
+        <v>1500</v>
+      </c>
+      <c r="B4" s="0">
+        <v>2</v>
+      </c>
+      <c r="C4" s="0">
+        <v>48</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1623.65</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="0">
+        <v>3000</v>
+      </c>
+      <c r="B5" s="0">
+        <v>4</v>
+      </c>
+      <c r="C5" s="0">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E5" s="6">
+        <v>3244.8</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="0">
+        <v>5000</v>
+      </c>
+      <c r="B6" s="0">
+        <v>2</v>
+      </c>
+      <c r="C6" s="0">
+        <v>48</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="E6" s="0">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s" s="11">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>